<commit_message>
Added API call for getting a list of screens (and well counts - in line with other screen list calls) of all screens which are the same/subsets of a specified screen
</commit_message>
<xml_diff>
--- a/c3_data/monomers.xlsx
+++ b/c3_data/monomers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janetnewman/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{082771B4-AA39-D14E-9BAF-D55BB865B606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BC5632-A8F3-D742-8F64-E215D5F92E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19240" yWindow="7580" windowWidth="27640" windowHeight="16940" xr2:uid="{900A7541-B87A-534B-8F97-383F01E320E5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="92">
   <si>
     <t>dextran 1500</t>
   </si>
@@ -160,13 +160,166 @@
   </si>
   <si>
     <t>propylene glycol</t>
+  </si>
+  <si>
+    <t>4-nonylphenyl-polyethylene glycol</t>
+  </si>
+  <si>
+    <t>poly(3-hydroxybutyric acid)</t>
+  </si>
+  <si>
+    <t>poly(acrylic acid-co-maleic acid)</t>
+  </si>
+  <si>
+    <t>polyacrylic acid 2100 sodium salt</t>
+  </si>
+  <si>
+    <t>polyacrylic acid 5100 sodium salt</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 1000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 10000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 12000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 1450</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 1500</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 15000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 200</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 2000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 20000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 250 diacid</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 300</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 3000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 3350</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 35000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 400</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 4000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 40000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 4600</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 600</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 6000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol 8000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol dimethyl ether 250</t>
+  </si>
+  <si>
+    <t>polyethylene glycol dimethyl ether 500</t>
+  </si>
+  <si>
+    <t>polyethylene glycol monomethyl ether 2000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol monomethyl ether 350</t>
+  </si>
+  <si>
+    <t>polyethylene glycol monomethyl ether 5000</t>
+  </si>
+  <si>
+    <t>polyethylene glycol monomethyl ether 550</t>
+  </si>
+  <si>
+    <t>polyethylene glycol monomethyl ether 750</t>
+  </si>
+  <si>
+    <t>polyethylene glycol monomethylether 1900</t>
+  </si>
+  <si>
+    <t>Polyethylene glycol nonylphenyl ether</t>
+  </si>
+  <si>
+    <t>polyoxometalate hexatungstotellurate (VI)</t>
+  </si>
+  <si>
+    <t>polypropylene glycol 425</t>
+  </si>
+  <si>
+    <t>polypropylene glycol P400</t>
+  </si>
+  <si>
+    <t>polyvinyl alcohol</t>
+  </si>
+  <si>
+    <t>polyvinylpyrrolidone K15</t>
+  </si>
+  <si>
+    <t>polyvinylpyrrolidone K25</t>
+  </si>
+  <si>
+    <t>sodium tripolyphosphate</t>
+  </si>
+  <si>
+    <t>detergent</t>
+  </si>
+  <si>
+    <t>additive</t>
+  </si>
+  <si>
+    <t>Acrylic acid-maleic acid</t>
+  </si>
+  <si>
+    <t>Acrylic acid</t>
+  </si>
+  <si>
+    <t>Note Av molecular weight 3000</t>
+  </si>
+  <si>
+    <t>for synthesis only! Very acidic!</t>
+  </si>
+  <si>
+    <t>Polymer</t>
+  </si>
+  <si>
+    <t>ethenol</t>
+  </si>
+  <si>
+    <t>1-Ethenylpyrrolidin-2-one</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -185,6 +338,24 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF4D5156"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -207,9 +378,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393771B8-AC60-9F46-A8E6-EC29FB5A53BF}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D22"/>
+      <selection activeCell="H56" sqref="H55:H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,7 +909,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -746,7 +920,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -757,7 +931,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -768,7 +942,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -779,7 +953,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -790,7 +964,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -801,7 +975,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
@@ -810,6 +984,453 @@
       </c>
       <c r="C23" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated monomer population script
</commit_message>
<xml_diff>
--- a/c3_data/monomers.xlsx
+++ b/c3_data/monomers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janetnewman/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i_am_\Documents\GIT_REPOS\C6Redux\c3_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BC5632-A8F3-D742-8F64-E215D5F92E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E10D5DE-2165-4CAF-BC9F-7CA685878F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19240" yWindow="7580" windowWidth="27640" windowHeight="16940" xr2:uid="{900A7541-B87A-534B-8F97-383F01E320E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{900A7541-B87A-534B-8F97-383F01E320E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -319,7 +319,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -342,20 +342,15 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF4D5156"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -381,9 +376,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,724 +713,726 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393771B8-AC60-9F46-A8E6-EC29FB5A53BF}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H56" sqref="H55:H56"/>
+      <selection activeCell="D64" sqref="A1:D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.1640625" customWidth="1"/>
+    <col min="1" max="1" width="46.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B24" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B25" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B33" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="B32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="B35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B38" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B40" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B39" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B40" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B42" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="B41" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B43" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="B42" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="B43" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="B44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="B45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="B46" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B48" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="B47" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B49" t="s">
-        <v>89</v>
-      </c>
-      <c r="C49" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="B48" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B50" t="s">
-        <v>89</v>
-      </c>
-      <c r="C50" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="B49" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B51" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="B50" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B52" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="B51" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B53" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="B52" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B54" t="s">
-        <v>89</v>
-      </c>
-      <c r="C54" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="B53" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B55" t="s">
-        <v>89</v>
-      </c>
-      <c r="C55" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="B54" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B56" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B55" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B57" t="s">
-        <v>89</v>
-      </c>
-      <c r="C57" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="B56" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B58" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B57" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B58" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B59" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B61" t="s">
-        <v>12</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="B60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="B61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>80</v>
-      </c>
-      <c r="B64" t="s">
-        <v>12</v>
-      </c>
-      <c r="C64" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B65" t="s">
-        <v>12</v>
-      </c>
-      <c r="C65" s="4" t="s">
+      <c r="B64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B65" s="2" t="s">
         <v>84</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1447,12 +1444,12 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1460,7 +1457,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1468,7 +1465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1476,7 +1473,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>